<commit_message>
tests adjusted as part of Connectathon 37 and results in spreadsheet
</commit_message>
<xml_diff>
--- a/postman-tests/FHIR Terminology Server API Testing Status C37.xlsx
+++ b/postman-tests/FHIR Terminology Server API Testing Status C37.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryantaustin/Projects/ecqm/cqf-measures-local/postman-tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89D34159-31DE-EB4B-A2CF-EE4207D7FAFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B834E7AE-383B-5A4C-9A6A-113FE7C0B21C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10920" yWindow="1440" windowWidth="24920" windowHeight="17500" activeTab="4" xr2:uid="{0D5B6508-2202-490B-81AD-3E791A748B4C}"/>
+    <workbookView xWindow="10920" yWindow="1440" windowWidth="24920" windowHeight="17500" activeTab="1" xr2:uid="{0D5B6508-2202-490B-81AD-3E791A748B4C}"/>
   </bookViews>
   <sheets>
     <sheet name="General Summary" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="OCL Results" sheetId="6" r:id="rId5"/>
     <sheet name="Requirements" sheetId="1" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,6 +32,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="954" uniqueCount="396">
   <si>
     <t>Requirement</t>
   </si>
@@ -771,13 +772,1671 @@
   </si>
   <si>
     <t>Actual Behavior</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FFCA3323"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>#</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCA3323"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FFCA3323"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>failure</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCA3323"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">                                </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FFCA3323"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>detail</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCA3323"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>                                                                                                                                                 </t>
+    </r>
+  </si>
+  <si>
+    <t>                                                                                                                                                                                                    </t>
+  </si>
+  <si>
+    <t> 01.  AssertionError                         Resource version contains 2.1.0                                                                                                                        </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                             </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7D7D7D"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>expected undefined to exist</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">                                                                                                                            </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                             </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7D7D7D"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>at assertion:2 in test-script</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">                                                                                                                          </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                             </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7D7D7D"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>inside "CodeSystem / CodeSystem 6:Search / SHALL / CodeSystem 6.3 Search by Identifier"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">                                                                </t>
+    </r>
+  </si>
+  <si>
+    <t> 02.  AssertionError                         Response status code is 200                                                                                                                            </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                             </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7D7D7D"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>expected 400 to equal 200</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">                                                                                                                              </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                             </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7D7D7D"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>at assertion:0 in test-script</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">                                                                                                                          </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                             </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7D7D7D"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>inside "CodeSystem / CodeSystem 6:Search / CodeSystem 7 Search (SHOULD) / CodeSystem 7.2 Search By ValueSet"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>                                           </t>
+    </r>
+  </si>
+  <si>
+    <t> 03.  TypeError                              Resource url is http://terminology.hl7.org/CodeSystem/allergyintolerance-clinical                                                                      </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                             </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7D7D7D"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>Cannot read properties of undefined (reading '0')</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">                                                                                                      </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                             </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7D7D7D"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>at assertion:1 in test-script</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">                                                                                                                          </t>
+    </r>
+  </si>
+  <si>
+    <t> 04.  TypeError                              Resource version is 0.5.0                                                                                                                              </t>
+  </si>
+  <si>
+    <t> 05.  TypeError                              Resource name is AllergyIntoleranceClinicalStatusCodes                                                                                                 </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                             </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7D7D7D"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>at assertion:3 in test-script</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">                                                                                                                          </t>
+    </r>
+  </si>
+  <si>
+    <t> 06.  TypeError                              Resource status is draft                                                                                                                               </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                             </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7D7D7D"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>at assertion:4 in test-script</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">                                                                                                                          </t>
+    </r>
+  </si>
+  <si>
+    <t> 07.  TypeError                              Resource experimental is false                                                                                                                         </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                             </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7D7D7D"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>at assertion:5 in test-script</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">                                                                                                                          </t>
+    </r>
+  </si>
+  <si>
+    <t> 08.  TypeError                              Resource publisher is FHIR Project team                                                                                                                </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                             </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7D7D7D"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>at assertion:6 in test-script</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">                                                                                                                          </t>
+    </r>
+  </si>
+  <si>
+    <t> 09.  TypeError                              Resource title is AllergyIntolerance Clinical Status Codes                                                                                             </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                             </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7D7D7D"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>at assertion:7 in test-script</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">                                                                                                                          </t>
+    </r>
+  </si>
+  <si>
+    <t> 10.  TypeError                              Resource type is CodeSystem                                                                                                                            </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                             </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7D7D7D"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>at assertion:8 in test-script</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">                                                                                                                          </t>
+    </r>
+  </si>
+  <si>
+    <t> 11.  AssertionError                         Resource url is http://terminology.hl7.org/CodeSystem/allergyintolerance-clinical                                                                      </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                             </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7D7D7D"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>expected 'http://www.ama-assn.org/go/cpt' to equal 'http://terminology.hl7.org/CodeSystem/allergyintolerance-clinical'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>                                 </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                             </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7D7D7D"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>inside "CodeSystem / CodeSystem 6:Search / CodeSystem 7 Search (SHOULD) / CodeSystem 7.3 Search By Measure"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">                                            </t>
+    </r>
+  </si>
+  <si>
+    <t> 12.  AssertionError                         Resource version is 4.0.1                                                                                                                              </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                             </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7D7D7D"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>expected '2024' to equal '4.0.1'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>                                                                                                                       </t>
+    </r>
+  </si>
+  <si>
+    <t> 13.  AssertionError                         Resource name is AllergyIntoleranceClinicalStatusCodes                                                                                                 </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                             </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7D7D7D"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>expected 'CPT' to equal 'AllergyIntoleranceClinicalStatusCodes'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">                                                                                        </t>
+    </r>
+  </si>
+  <si>
+    <t> 14.  AssertionError                         Resource status is draft                                                                                                                               </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                             </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7D7D7D"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>expected 'active' to equal 'draft'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>                                                                                                                     </t>
+    </r>
+  </si>
+  <si>
+    <t> 15.  AssertionError                         Resource publisher is FHIR Project team                                                                                                                </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                             </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7D7D7D"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>expected undefined to equal 'FHIR Project team'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">                                                                                                        </t>
+    </r>
+  </si>
+  <si>
+    <t> 16.  AssertionError                         Resource title is AllergyIntolerance Clinical Status Codes                                                                                             </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                             </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7D7D7D"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>expected 'Current Procedural Terminology' to equal 'AllergyIntolerance Clinical Status Codes'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">                                                          </t>
+    </r>
+  </si>
+  <si>
+    <t> 17.  AssertionError                         Resource type is Measure                                                                                                                               </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                             </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7D7D7D"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>expected undefined to equal 'Measure'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">                                                                                                                  </t>
+    </r>
+  </si>
+  <si>
+    <t> 18.  TypeError                              Resource url is http://terminology.hl7.org/CodeSystem/allergyintolerance-clinical                                                                      </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                             </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7D7D7D"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>inside "CodeSystem / CodeSystem 6:Search / CodeSystem 7 Search (SHOULD) / CodeSystem 7.4 Search By Library"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">                                            </t>
+    </r>
+  </si>
+  <si>
+    <t> 19.  TypeError                              Resource version is 4.0.1                                                                                                                              </t>
+  </si>
+  <si>
+    <t> 20.  TypeError                              Resource name is AllergyIntoleranceClinicalStatusCodes                                                                                                 </t>
+  </si>
+  <si>
+    <t> 21.  TypeError                              Resource status is draft                                                                                                                               </t>
+  </si>
+  <si>
+    <t> 22.  TypeError                              Resource experimental is false                                                                                                                         </t>
+  </si>
+  <si>
+    <t> 23.  TypeError                              Resource publisher is FHIR Project team                                                                                                                </t>
+  </si>
+  <si>
+    <t> 24.  TypeError                              Resource title is AllergyIntolerance Clinical Status Codes                                                                                             </t>
+  </si>
+  <si>
+    <t> 25.  TypeError                              Resource type is Library                                                                                                                               </t>
+  </si>
+  <si>
+    <t> 26.  TypeError                              Resource url is http://terminology.hl7.org/CodeSystem/allergyintolerance-clinical                                                                      </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                             </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7D7D7D"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>inside "CodeSystem / CodeSystem 6:Search / CodeSystem 7 Search (SHOULD) / CodeSystem 7.5 Search By Artifact"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>                                           </t>
+    </r>
+  </si>
+  <si>
+    <t> 27.  TypeError                              Resource version is 4.0.1                                                                                                                              </t>
+  </si>
+  <si>
+    <t> 28.  TypeError                              Resource name is AllergyIntoleranceClinicalStatusCodes                                                                                                 </t>
+  </si>
+  <si>
+    <t> 29.  TypeError                              Resource status is draft                                                                                                                               </t>
+  </si>
+  <si>
+    <t> 30.  TypeError                              Resource experimental is false                                                                                                                         </t>
+  </si>
+  <si>
+    <t> 31.  TypeError                              Resource publisher is FHIR Project team                                                                                                                </t>
+  </si>
+  <si>
+    <t> 32.  TypeError                              Resource title is AllergyIntolerance Clinical Status Codes                                                                                             </t>
+  </si>
+  <si>
+    <t> 33.  TypeError                              Resource type is Artifact                                                                                                                              </t>
+  </si>
+  <si>
+    <t> 34.  TypeError                              Shareable profile is present in meta                                                                                                                   </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                             </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7D7D7D"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>Cannot read properties of undefined (reading 'profile')</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">                                                                                                </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                             </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7D7D7D"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>inside "ValueSet / Representation / ValueSet 1 Shareable / ValueSet 1.2 Shareable (THO)"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>                                                               </t>
+    </r>
+  </si>
+  <si>
+    <t> 35.  AssertionError                         Publishable profile is present in meta                                                                                                                 </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                             </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7D7D7D"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>expected [ Array(1) ] to include 'http://hl7.org/fhir/us/cqfmeasures/StructureDefinition/publishable-valueset-cqfm'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">                                    </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                             </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7D7D7D"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>inside "ValueSet / Representation / ValueSet 6 Publishable / ValueSet 6.1 Publishable (Ballot-bound)"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">                                                  </t>
+    </r>
+  </si>
+  <si>
+    <t> 36.  AssertionError                         LastReviewDate is 2022-12-15                                                                                                                           </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                             </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7D7D7D"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>lastReviewDate error: expected '2024-06-03' to equal '2022-12-15'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">                                                                                      </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                             </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7D7D7D"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>at assertion:9 in test-script</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">                                                                                                                          </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                             </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7D7D7D"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>inside "ValueSet / Representation / ValueSet 6 Publishable / ValueSet 6.5 Publishable (Authored)"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">                                                      </t>
+    </r>
+  </si>
+  <si>
+    <t> 37.  AssertionError                         LastReviewDate is 2023-02-17                                                                                                                           </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                             </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7D7D7D"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>lastReviewDate error: expected '2024-02-06' to equal '2023-02-17'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">                                                                                      </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                             </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7D7D7D"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>inside "ValueSet / Representation / ValueSet 6 Publishable / ValueSet 6.6 Publishable with Keywords (Authored)"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">                                        </t>
+    </r>
+  </si>
+  <si>
+    <t> 38.  AssertionError                         Publisher is TJC EH Author                                                                                                                             </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                             </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7D7D7D"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>Publisher error: expected 'TJC EH Steward' to equal 'TJC EH Author'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">                                                                                    </t>
+    </r>
+  </si>
+  <si>
+    <t> 39.  AssertionError                         Effective Date extension returns valueDateTime                                                                                                         </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                             </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7D7D7D"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>EffectiveDate error: expected undefined to equal '2023-02-17'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">                                                                                          </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                             </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7D7D7D"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>inside "ValueSet / Representation / ValueSet 6 Publishable / ValueSet 6.8 Publishable Value Set EffectiveDate uses valueDateTime"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">                      </t>
+    </r>
+  </si>
+  <si>
+    <t> 40.  AssertionError                         Response status code is 200                                                                                                                            </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                             </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7D7D7D"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>inside "ValueSet / ValueSet 8 Search / SHALL / ValueSet 8.6 Search By Status"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">                                                                          </t>
+    </r>
+  </si>
+  <si>
+    <t> 41.  AssertionError                         Total is greater than 0                                                                                                                                </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                             </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7D7D7D"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>expected undefined to be a number or a date</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">                                                                                                            </t>
+    </r>
+  </si>
+  <si>
+    <t> 42.  AssertionError                         Response status code is 200                                                                                                                            </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                             </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7D7D7D"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>inside "ValueSet / ValueSet 10 ValidateCode / ValueSet 10.5 Validate Code With Code"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>                                                                   </t>
+    </r>
+  </si>
+  <si>
+    <t> 43.  AssertionError                         Resource type is Parameters                                                                                                                            </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                             </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7D7D7D"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>expected 'OperationOutcome' to equal 'Parameters'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">                                                                                                      </t>
+    </r>
+  </si>
+  <si>
+    <t> 44.  TypeError                              Parameters contain a result of true                                                                                                                    </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                             </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7D7D7D"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>Cannot read properties of undefined (reading 'find')</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>                                                                                                   </t>
+    </r>
+  </si>
+  <si>
+    <t> 45.  TypeError                              Parameters contain a display of Goldmann three-mirror contact lens (physical object)                                                                   </t>
+  </si>
+  <si>
+    <t> 46.  AssertionError                         Response status code is 200                                                                                                                            </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                             </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7D7D7D"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>inside "ValueSet / Expand / ValueSet 12 Post / ValueSet 12.4 POST Expand With Limited Expansion"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>                                                       </t>
+    </r>
+  </si>
+  <si>
+    <t> 47.  AssertionError                         Test that version is present                                                                                                                           </t>
+  </si>
+  <si>
+    <t> 48.  AssertionError                         Name is present                                                                                                                                        </t>
+  </si>
+  <si>
+    <t> 49.  AssertionError                         Status is present                                                                                                                                      </t>
+  </si>
+  <si>
+    <t> 50.  AssertionError                         Publisher is present                                                                                                                                   </t>
+  </si>
+  <si>
+    <t> 51.  AssertionError                         Title is present                                                                                                                                       </t>
+  </si>
+  <si>
+    <t> 52.  AssertionError                         Date is present                                                                                                                                        </t>
+  </si>
+  <si>
+    <t> 53.  AssertionError                         Expansion is present                                                                                                                                   </t>
+  </si>
+  <si>
+    <t> 54.  AssertionError                         Response status code is 200                                                                                                                            </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                             </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7D7D7D"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>inside "ValueSet / Expand / ValueSet 12 Post / ValueSet 12.5 POST Expand With Default To Latest Version"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>                                               </t>
+    </r>
+  </si>
+  <si>
+    <t> 55.  AssertionError                         Test that version is present                                                                                                                           </t>
+  </si>
+  <si>
+    <t> 56.  AssertionError                         Name is present                                                                                                                                        </t>
+  </si>
+  <si>
+    <t> 57.  AssertionError                         Status is present                                                                                                                                      </t>
+  </si>
+  <si>
+    <t> 58.  AssertionError                         Publisher is present                                                                                                                                   </t>
+  </si>
+  <si>
+    <t> 59.  AssertionError                         Title is present                                                                                                                                       </t>
+  </si>
+  <si>
+    <t> 60.  AssertionError                         Date is present                                                                                                                                        </t>
+  </si>
+  <si>
+    <t> 61.  AssertionError                         Expansion is present                                                                                                                                   </t>
+  </si>
+  <si>
+    <t> 62.  AssertionError                         Response status code is 200                                                                                                                            </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                             </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7D7D7D"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>inside "ValueSet / Expand / ValueSet 12 Post / ValueSet 12.10 POST Expand With Check Canonical Version"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">                                                </t>
+    </r>
+  </si>
+  <si>
+    <t> 63.  AssertionError                         Test that version is present                                                                                                                           </t>
+  </si>
+  <si>
+    <t> 64.  AssertionError                         Name is present                                                                                                                                        </t>
+  </si>
+  <si>
+    <t> 65.  AssertionError                         Status is present                                                                                                                                      </t>
+  </si>
+  <si>
+    <t> 66.  AssertionError                         Publisher is present                                                                                                                                   </t>
+  </si>
+  <si>
+    <t> 67.  AssertionError                         Title is present                                                                                                                                       </t>
+  </si>
+  <si>
+    <t> 68.  AssertionError                         Date is present                                                                                                                                        </t>
+  </si>
+  <si>
+    <t> 69.  AssertionError                         Expansion is present                                                                                                                                   </t>
+  </si>
+  <si>
+    <t> 70.  AssertionError                         Response status code is 200                                                                                                                            </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                             </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7D7D7D"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>inside "ValueSet / Expand / ValueSet 12 Post / ValueSet 12.11 POST Expand With Force Canonoical Version"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>                                               </t>
+    </r>
+  </si>
+  <si>
+    <t> 71.  AssertionError                         Test that version is present                                                                                                                           </t>
+  </si>
+  <si>
+    <t> 72.  AssertionError                         Name is present                                                                                                                                        </t>
+  </si>
+  <si>
+    <t> 73.  AssertionError                         Status is present                                                                                                                                      </t>
+  </si>
+  <si>
+    <t> 74.  AssertionError                         Publisher is present                                                                                                                                   </t>
+  </si>
+  <si>
+    <t> 75.  AssertionError                         Title is present                                                                                                                                       </t>
+  </si>
+  <si>
+    <t> 76.  AssertionError                         Date is present                                                                                                                                        </t>
+  </si>
+  <si>
+    <t> 77.  AssertionError                         Expansion is present                                                                                                                                   </t>
+  </si>
+  <si>
+    <t> 78.  AssertionError                         Code is present                                                                                                                                        </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                             </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7D7D7D"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>inside "Quality Program / Manifest Support 6 / Quality Program Manifest Support 6.5 Expand With Url"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>                                                   </t>
+    </r>
+  </si>
+  <si>
+    <t> 79.  AssertionError                         Response status code is 200 or 201                                                                                                                     </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                             </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7D7D7D"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>expected 400 to be one of [ 200, 201 ]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>                                                                                                                 </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                             </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7D7D7D"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>inside "Quality Program / Release 8 / Quality Program Release 8.1 Create Draft"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">                                                                        </t>
+    </r>
+  </si>
+  <si>
+    <t> 80.  AssertionError                         Resource Type should be transaction-response                                                                                                           </t>
+  </si>
+  <si>
+    <t> 81.  AssertionError                         Test that id is not empty                                                                                                                              </t>
+  </si>
+  <si>
+    <t> 82.  AssertionError                         Response status code is 200 or 201                                                                                                                     </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                             </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7D7D7D"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>inside "Quality Program / Release 8 / Quality Program Release 8.2 Update Draft"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">                                                                        </t>
+    </r>
+  </si>
+  <si>
+    <t> 83.  AssertionError                         Resource Type should be transaction-response                                                                                                           </t>
+  </si>
+  <si>
+    <t> 84.  AssertionError                         Test that id is not empty                                                                                                                              </t>
+  </si>
+  <si>
+    <t> 85.  AssertionError                         Response status code is 200                                                                                                                            </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                             </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7D7D7D"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>expected 400 to equal '200'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">                                                                                                                            </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                             </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7D7D7D"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>inside "Quality Program / Release 8 / Quality Program Release 8.3 Release Library"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>                                                                     </t>
+    </r>
+  </si>
+  <si>
+    <t> 86.  AssertionError                         Resource Type should be transaction-response                                                                                                           </t>
+  </si>
+  <si>
+    <t> 87.  AssertionError                         Test that id is not empty                                                                                                                              </t>
+  </si>
+  <si>
+    <t> 88.  AssertionError                         Status is active                                                                                                                                       </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                             </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7D7D7D"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>expected undefined to equal 'active'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>                                                                                                                   </t>
+    </r>
+  </si>
+  <si>
+    <t> 89.  AssertionError                         Response status code is 200                                                                                                                            </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                             </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7D7D7D"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>inside "Quality Program / Release 8 / Quality Program Release 8.4 Retire Library"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">                                                                      </t>
+    </r>
+  </si>
+  <si>
+    <t> 90.  AssertionError                         Resource Type should be transaction-response                                                                                                           </t>
+  </si>
+  <si>
+    <t> 91.  AssertionError                         Test that id is not empty                                                                                                                              </t>
+  </si>
+  <si>
+    <t> 92.  AssertionError                         Status is retired                                                                                                                                      </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                             </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7D7D7D"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>expected undefined to equal 'retired'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">                                                                                                                  </t>
+    </r>
+  </si>
+  <si>
+    <t> 93.  TypeError                              Test that return entry[0] is resourceType == Parameters.                                                                                               </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                             </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7D7D7D"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>Cannot read properties of undefined (reading 'resourceType')</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>                                                                                           </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                             </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7D7D7D"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>inside "Server / Server 2 Batch Operations / Server 2 Batch CodeSystem Read"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>                                                                           </t>
+    </r>
+  </si>
+  <si>
+    <t> 94.  TypeError                              Test that validateCode returns true - code exists.                                                                                                     </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                             </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7D7D7D"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>inside "Server / Server 2 Batch Operations / Server 2 Batch CodeSystem Read"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>       </t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -827,6 +2486,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFCA3323"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FFCA3323"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF7D7D7D"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -849,7 +2533,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -865,6 +2549,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -884,9 +2571,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -924,7 +2611,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1030,7 +2717,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1172,7 +2859,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1183,7 +2870,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1260,7 +2947,7 @@
         <v>692</v>
       </c>
       <c r="G3" s="5">
-        <f t="shared" ref="G3:G6" si="0">INT((F3-E3)/F3*100)</f>
+        <f t="shared" ref="G3:G5" si="0">INT((F3-E3)/F3*100)</f>
         <v>48</v>
       </c>
       <c r="H3" s="5"/>
@@ -1320,16 +3007,9 @@
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
-      <c r="E6" s="5">
-        <v>337</v>
-      </c>
-      <c r="F6" s="5">
-        <v>702</v>
-      </c>
-      <c r="G6" s="5">
-        <f t="shared" si="0"/>
-        <v>51</v>
-      </c>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
       <c r="H6" s="5"/>
     </row>
   </sheetData>
@@ -1345,10 +3025,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75784DF6-A0E2-BD4F-B6C3-4DF6225DD89B}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C471"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A471"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1357,15 +3037,2360 @@
     <col min="2" max="2" width="29.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="7" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
-        <v>240</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>241</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>242</v>
+    <row r="1" spans="1:3" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="C1" s="8"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="11" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="11" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="11" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="11" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="11" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="11" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="11" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="11" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="11" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" s="11" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" s="11" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" s="11" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" s="11" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" s="11" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" s="11" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" s="11" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" s="11" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" s="11" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" s="11" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" s="11" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" s="11" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" s="11" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" s="11" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" s="11" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" s="11" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" s="11" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43" s="11" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" s="11" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45" s="11" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46" s="11" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A47" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A48" s="11" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" s="11" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" s="11" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51" s="11" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A53" s="11" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54" s="11" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A55" s="11" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A56" s="11" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A57" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A58" s="11" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A59" s="11" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A60" s="11" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A61" s="11" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A62" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A63" s="11" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A64" s="11" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A65" s="11" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A66" s="11" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A67" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A68" s="11" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A69" s="11" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A70" s="11" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A71" s="11" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A72" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A73" s="11" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A74" s="11" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A75" s="11" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A76" s="11" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A77" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A78" s="11" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A79" s="11" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A80" s="11" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A81" s="11" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A82" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A83" s="11" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A84" s="11" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A85" s="11" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A86" s="11" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A87" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A88" s="11" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A89" s="11" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A90" s="11" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A91" s="11" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A92" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A93" s="11" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A94" s="11" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A95" s="11" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A96" s="11" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A97" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A98" s="11" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A99" s="11" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A100" s="11" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A101" s="11" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A102" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A103" s="11" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A104" s="11" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A105" s="11" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A106" s="11" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A107" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A108" s="11" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A109" s="11" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A110" s="11" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A111" s="11" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A112" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A113" s="11" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A114" s="11" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A115" s="11" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A116" s="11" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A117" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A118" s="11" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A119" s="11" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A120" s="11" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A121" s="11" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A122" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A123" s="11" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A124" s="11" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A125" s="11" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A126" s="11" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A127" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A128" s="11" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A129" s="11" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A130" s="11" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A131" s="11" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A132" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A133" s="11" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A134" s="11" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A135" s="11" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A136" s="11" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A137" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A138" s="11" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A139" s="11" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A140" s="11" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A141" s="11" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A142" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A143" s="11" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A144" s="11" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A145" s="11" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A146" s="11" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A147" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A148" s="11" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A149" s="11" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A150" s="11" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A151" s="11" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A152" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A153" s="11" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A154" s="11" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A155" s="11" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A156" s="11" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A157" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A158" s="11" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A159" s="11" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A160" s="11" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A161" s="11" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A162" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A163" s="11" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A164" s="11" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A165" s="11" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A166" s="11" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A167" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A168" s="11" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A169" s="11" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A170" s="11" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A171" s="11" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A172" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A173" s="11" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A174" s="11" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A175" s="11" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A176" s="11" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A177" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A178" s="11" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A179" s="11" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A180" s="11" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A181" s="11" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A182" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A183" s="11" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A184" s="11" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A185" s="11" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A186" s="11" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A187" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A188" s="11" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A189" s="11" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A190" s="11" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A191" s="11" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A192" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A193" s="11" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A194" s="11" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A195" s="11" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A196" s="11" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A197" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A198" s="11" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A199" s="11" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A200" s="11" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A201" s="11" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A202" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A203" s="11" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A204" s="11" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A205" s="11" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A206" s="11" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A207" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A208" s="11" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A209" s="11" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A210" s="11" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A211" s="11" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A212" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A213" s="11" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A214" s="11" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A215" s="11" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A216" s="11" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A217" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A218" s="11" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A219" s="11" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A220" s="11" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="221" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A221" s="11" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A222" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="223" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A223" s="11" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A224" s="11" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A225" s="11" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A226" s="11" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A227" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A228" s="11" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A229" s="11" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A230" s="11" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="231" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A231" s="11" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A232" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A233" s="11" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A234" s="11" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="235" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A235" s="11" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="236" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A236" s="11" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="237" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A237" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="238" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A238" s="11" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="239" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A239" s="11" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="240" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A240" s="11" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="241" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A241" s="11" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="242" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A242" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="243" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A243" s="11" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="244" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A244" s="11" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="245" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A245" s="11" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="246" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A246" s="11" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="247" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A247" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="248" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A248" s="11" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="249" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A249" s="11" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="250" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A250" s="11" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="251" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A251" s="11" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="252" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A252" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="253" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A253" s="11" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="254" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A254" s="11" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="255" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A255" s="11" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="256" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A256" s="11" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="257" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A257" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="258" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A258" s="11" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="259" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A259" s="11" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="260" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A260" s="11" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="261" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A261" s="11" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="262" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A262" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="263" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A263" s="11" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="264" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A264" s="11" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="265" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A265" s="11" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="266" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A266" s="11" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="267" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A267" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="268" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A268" s="11" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="269" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A269" s="11" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="270" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A270" s="11" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="271" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A271" s="11" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="272" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A272" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="273" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A273" s="11" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="274" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A274" s="11" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="275" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A275" s="11" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="276" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A276" s="11" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="277" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A277" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="278" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A278" s="11" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="279" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A279" s="11" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="280" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A280" s="11" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="281" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A281" s="11" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="282" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A282" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="283" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A283" s="11" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="284" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A284" s="11" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="285" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A285" s="11" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="286" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A286" s="11" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="287" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A287" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="288" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A288" s="11" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="289" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A289" s="11" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="290" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A290" s="11" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="291" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A291" s="11" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="292" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A292" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="293" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A293" s="11" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="294" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A294" s="11" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="295" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A295" s="11" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="296" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A296" s="11" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="297" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A297" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="298" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A298" s="11" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="299" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A299" s="11" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="300" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A300" s="11" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="301" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A301" s="11" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="302" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A302" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="303" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A303" s="11" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="304" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A304" s="11" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="305" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A305" s="11" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="306" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A306" s="11" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="307" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A307" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="308" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A308" s="11" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="309" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A309" s="11" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="310" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A310" s="11" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="311" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A311" s="11" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="312" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A312" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="313" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A313" s="11" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="314" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A314" s="11" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="315" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A315" s="11" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="316" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A316" s="11" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="317" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A317" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="318" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A318" s="11" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="319" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A319" s="11" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="320" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A320" s="11" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="321" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A321" s="11" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="322" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A322" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="323" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A323" s="11" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="324" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A324" s="11" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="325" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A325" s="11" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="326" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A326" s="11" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="327" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A327" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="328" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A328" s="11" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="329" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A329" s="11" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="330" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A330" s="11" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="331" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A331" s="11" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="332" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A332" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="333" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A333" s="11" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="334" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A334" s="11" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="335" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A335" s="11" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="336" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A336" s="11" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="337" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A337" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="338" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A338" s="11" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="339" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A339" s="11" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="340" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A340" s="11" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="341" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A341" s="11" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="342" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A342" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="343" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A343" s="11" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="344" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A344" s="11" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="345" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A345" s="11" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="346" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A346" s="11" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="347" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A347" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="348" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A348" s="11" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="349" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A349" s="11" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="350" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A350" s="11" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="351" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A351" s="11" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="352" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A352" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="353" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A353" s="11" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="354" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A354" s="11" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="355" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A355" s="11" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="356" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A356" s="11" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="357" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A357" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="358" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A358" s="11" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="359" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A359" s="11" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="360" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A360" s="11" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="361" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A361" s="11" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="362" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A362" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="363" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A363" s="11" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="364" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A364" s="11" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="365" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A365" s="11" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="366" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A366" s="11" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="367" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A367" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="368" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A368" s="11" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="369" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A369" s="11" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="370" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A370" s="11" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="371" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A371" s="11" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="372" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A372" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="373" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A373" s="11" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="374" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A374" s="11" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="375" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A375" s="11" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="376" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A376" s="11" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="377" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A377" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="378" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A378" s="11" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="379" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A379" s="11" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="380" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A380" s="11" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="381" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A381" s="11" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="382" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A382" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="383" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A383" s="11" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="384" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A384" s="11" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="385" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A385" s="11" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="386" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A386" s="11" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="387" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A387" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="388" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A388" s="11" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="389" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A389" s="11" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="390" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A390" s="11" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="391" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A391" s="11" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="392" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A392" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="393" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A393" s="11" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="394" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A394" s="11" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="395" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A395" s="11" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="396" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A396" s="11" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="397" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A397" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="398" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A398" s="11" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="399" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A399" s="11" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="400" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A400" s="11" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="401" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A401" s="11" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="402" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A402" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="403" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A403" s="11" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="404" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A404" s="11" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="405" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A405" s="11" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="406" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A406" s="11" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="407" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A407" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="408" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A408" s="11" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="409" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A409" s="11" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="410" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A410" s="11" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="411" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A411" s="11" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="412" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A412" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="413" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A413" s="11" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="414" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A414" s="11" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="415" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A415" s="11" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="416" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A416" s="11" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="417" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A417" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="418" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A418" s="11" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="419" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A419" s="11" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="420" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A420" s="11" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="421" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A421" s="11" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="422" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A422" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="423" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A423" s="11" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="424" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A424" s="11" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="425" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A425" s="11" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="426" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A426" s="11" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="427" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A427" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="428" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A428" s="11" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="429" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A429" s="11" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="430" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A430" s="11" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="431" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A431" s="11" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="432" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A432" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="433" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A433" s="11" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="434" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A434" s="11" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="435" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A435" s="11" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="436" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A436" s="11" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="437" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A437" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="438" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A438" s="11" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="439" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A439" s="11" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="440" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A440" s="11" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="441" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A441" s="11" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="442" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A442" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="443" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A443" s="11" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="444" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A444" s="11" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="445" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A445" s="11" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="446" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A446" s="11" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="447" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A447" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="448" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A448" s="11" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="449" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A449" s="11" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="450" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A450" s="11" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="451" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A451" s="11" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="452" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A452" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="453" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A453" s="11" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="454" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A454" s="11" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="455" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A455" s="11" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="456" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A456" s="11" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="457" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A457" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="458" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A458" s="11" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="459" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A459" s="11" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="460" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A460" s="11" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="461" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A461" s="11" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="462" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A462" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="463" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A463" s="11" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="464" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A464" s="11" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="465" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A465" s="11" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="466" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A466" s="11" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="467" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A467" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="468" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A468" s="11" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="469" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A469" s="11" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="470" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A470" s="11" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="471" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A471" s="11" t="s">
+        <v>395</v>
       </c>
     </row>
   </sheetData>
@@ -1429,7 +5454,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4EBFDE9-7534-A148-BD0A-7F5C2430A8CC}">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>

</xml_diff>